<commit_message>
Adding triggerAgent, getInventoryReservationList, cancelReservation, processOrderPayments
</commit_message>
<xml_diff>
--- a/src/main/resources/TestItems_STH.xlsx
+++ b/src/main/resources/TestItems_STH.xlsx
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AUTOMATION\OMSAutomation\src\main\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10305" windowHeight="6180"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13720" windowHeight="2850"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -185,17 +181,17 @@
     <t>Order.EnterpriseCode</t>
   </si>
   <si>
+    <t>OrderLine.ShipNode</t>
+  </si>
+  <si>
     <t>FCVColombia</t>
-  </si>
-  <si>
-    <t>OrderLine.ShipNode</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -206,6 +202,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF202124"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF505253"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -236,11 +238,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,30 +526,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="26.85546875" customWidth="1"/>
-    <col min="5" max="5" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.5703125" customWidth="1"/>
-    <col min="7" max="7" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="31.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="26.81640625" customWidth="1"/>
+    <col min="5" max="5" width="27.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.54296875" customWidth="1"/>
+    <col min="7" max="7" width="26.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.81640625" customWidth="1"/>
     <col min="9" max="9" width="40" customWidth="1"/>
-    <col min="10" max="10" width="23.7109375" customWidth="1"/>
-    <col min="11" max="11" width="38.42578125" customWidth="1"/>
+    <col min="10" max="10" width="23.7265625" customWidth="1"/>
+    <col min="11" max="11" width="38.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -563,7 +566,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -576,21 +579,21 @@
       <c r="D3" t="s">
         <v>39</v>
       </c>
-      <c r="E3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E3" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -625,15 +628,15 @@
         <v>34</v>
       </c>
       <c r="L7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>100732</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
         <v>49</v>
@@ -660,13 +663,13 @@
         <v>3</v>
       </c>
       <c r="K8">
-        <v>457</v>
+        <v>1111</v>
       </c>
       <c r="L8">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>121486</v>
       </c>
@@ -704,7 +707,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>121486</v>
       </c>
@@ -742,17 +745,17 @@
         <v>457</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -781,7 +784,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>40</v>
       </c>
@@ -810,17 +813,17 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -840,7 +843,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>44</v>
       </c>
@@ -860,7 +863,7 @@
         <v>1914</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>2</v>
       </c>

</xml_diff>